<commit_message>
fix filter institution type
</commit_message>
<xml_diff>
--- a/Institutions_Final.xlsx
+++ b/Institutions_Final.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2437" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="641">
   <si>
     <t>Field</t>
   </si>
@@ -1950,6 +1950,9 @@
   </si>
   <si>
     <t>Vysoké školy</t>
+  </si>
+  <si>
+    <t>SumShare</t>
   </si>
 </sst>
 </file>
@@ -25489,10 +25492,10 @@
   <dimension ref="A1:N290"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D183" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E110" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G290" sqref="G290"/>
+      <selection pane="bottomRight" activeCell="L136" sqref="L136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25546,6 +25549,9 @@
       </c>
       <c r="M1" s="16" t="s">
         <v>635</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>